<commit_message>
news for control firm
</commit_message>
<xml_diff>
--- a/Version3/Raw/AR.xlsx
+++ b/Version3/Raw/AR.xlsx
@@ -5,26 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TC\Desktop\DI\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\financerpa\Desktop\PaperPilot\Version3\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD3E0F8-7C17-4A0A-9D8D-03EB99A9E13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796ECC86-2E18-413C-991F-1F510153248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="14440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表4" sheetId="8" r:id="rId1"/>
-    <sheet name="RPAfromAR" sheetId="1" r:id="rId2"/>
-    <sheet name="IndustryHaveRPA" sheetId="2" r:id="rId3"/>
-    <sheet name="Ctd" sheetId="4" r:id="rId4"/>
+    <sheet name="Control" sheetId="9" r:id="rId2"/>
+    <sheet name="RPAfromAR" sheetId="1" r:id="rId3"/>
+    <sheet name="IndustryHaveRPA" sheetId="2" r:id="rId4"/>
+    <sheet name="Ctd" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Ctd!$B$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RPAfromAR!$A$1:$F$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Ctd!$B$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RPAfromAR!$A$1:$F$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="35" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="272">
   <si>
     <t>代號</t>
   </si>
@@ -610,6 +611,275 @@
   </si>
   <si>
     <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>譜瑞-KY</t>
+  </si>
+  <si>
+    <t>穩懋</t>
+  </si>
+  <si>
+    <t>界霖</t>
+  </si>
+  <si>
+    <t>中磊</t>
+  </si>
+  <si>
+    <t>智捷</t>
+  </si>
+  <si>
+    <t>遠傳</t>
+  </si>
+  <si>
+    <t>光環</t>
+  </si>
+  <si>
+    <t>台林</t>
+  </si>
+  <si>
+    <t>前鼎</t>
+  </si>
+  <si>
+    <t>兆勁</t>
+  </si>
+  <si>
+    <t>亞光</t>
+  </si>
+  <si>
+    <t>銘旺科</t>
+  </si>
+  <si>
+    <t>欣普羅</t>
+  </si>
+  <si>
+    <t>友達</t>
+  </si>
+  <si>
+    <t>晶采</t>
+  </si>
+  <si>
+    <t>安可</t>
+  </si>
+  <si>
+    <t>彩晶</t>
+  </si>
+  <si>
+    <t>全國電</t>
+  </si>
+  <si>
+    <t>聯強</t>
+  </si>
+  <si>
+    <t>傳奇</t>
+  </si>
+  <si>
+    <t>訊連</t>
+  </si>
+  <si>
+    <t>三商電</t>
+  </si>
+  <si>
+    <t>實威</t>
+  </si>
+  <si>
+    <t>寶碩</t>
+  </si>
+  <si>
+    <t>凌群</t>
+  </si>
+  <si>
+    <t>緯軟</t>
+  </si>
+  <si>
+    <t>中菲</t>
+  </si>
+  <si>
+    <t>國眾</t>
+  </si>
+  <si>
+    <t>上奇</t>
+  </si>
+  <si>
+    <t>潤泰全</t>
+  </si>
+  <si>
+    <t>和泰車</t>
+  </si>
+  <si>
+    <t>群光</t>
+  </si>
+  <si>
+    <t>希華</t>
+  </si>
+  <si>
+    <t>良維</t>
+  </si>
+  <si>
+    <t>翔名</t>
+  </si>
+  <si>
+    <t>晟鈦</t>
+  </si>
+  <si>
+    <t>健策</t>
+  </si>
+  <si>
+    <t>寶得利</t>
+  </si>
+  <si>
+    <t>蜜望實</t>
+  </si>
+  <si>
+    <t>瓦城</t>
+  </si>
+  <si>
+    <t>台塑</t>
+  </si>
+  <si>
+    <t>勤益控</t>
+  </si>
+  <si>
+    <t>中石化</t>
+  </si>
+  <si>
+    <t>海悅</t>
+  </si>
+  <si>
+    <t>龍巖</t>
+  </si>
+  <si>
+    <t>福懋</t>
+  </si>
+  <si>
+    <t>南紡</t>
+  </si>
+  <si>
+    <t>大宇</t>
+  </si>
+  <si>
+    <t>新紡</t>
+  </si>
+  <si>
+    <t>嘉裕</t>
+  </si>
+  <si>
+    <t>東隆興</t>
+  </si>
+  <si>
+    <t>宏和</t>
+  </si>
+  <si>
+    <t>宜進</t>
+  </si>
+  <si>
+    <t>國喬</t>
+  </si>
+  <si>
+    <t>強盛</t>
+  </si>
+  <si>
+    <t>桂盟</t>
+  </si>
+  <si>
+    <t>巨大</t>
+  </si>
+  <si>
+    <t>大同</t>
+  </si>
+  <si>
+    <t>士電</t>
+  </si>
+  <si>
+    <t>伸興</t>
+  </si>
+  <si>
+    <t>亞德客-KY</t>
+  </si>
+  <si>
+    <t>謚源</t>
+  </si>
+  <si>
+    <t>基亞</t>
+  </si>
+  <si>
+    <t>皇將</t>
+  </si>
+  <si>
+    <t>慧智</t>
+  </si>
+  <si>
+    <t>東友</t>
+  </si>
+  <si>
+    <t>奇鋐</t>
+  </si>
+  <si>
+    <t>精元</t>
+  </si>
+  <si>
+    <t>銘異</t>
+  </si>
+  <si>
+    <t>歐格</t>
+  </si>
+  <si>
+    <t>新普</t>
+  </si>
+  <si>
+    <t>鼎翰</t>
+  </si>
+  <si>
+    <t>濱川</t>
+  </si>
+  <si>
+    <t>皇翔</t>
+  </si>
+  <si>
+    <t>台肥</t>
+  </si>
+  <si>
+    <t>展宇</t>
+  </si>
+  <si>
+    <t>旭隼</t>
+  </si>
+  <si>
+    <t>東科-KY</t>
+  </si>
+  <si>
+    <t>億豐</t>
+  </si>
+  <si>
+    <t>台船</t>
+  </si>
+  <si>
+    <t>華航</t>
+  </si>
+  <si>
+    <t>長榮</t>
+  </si>
+  <si>
+    <t>建新國際</t>
+  </si>
+  <si>
+    <t>聯詠</t>
+  </si>
+  <si>
+    <t>京鼎</t>
+  </si>
+  <si>
+    <t>台積電</t>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ec.ltn.com.tw/article/breakingnews/4317811</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,7 +887,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,6 +900,14 @@
       <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -650,19 +928,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1886,7 +2167,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D407809D-7623-43EE-9180-906AACDD752E}" name="樞紐分析表4" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D407809D-7623-43EE-9180-906AACDD752E}" name="樞紐分析表4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H134" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -2741,7 +3022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA41934E-79BE-4978-BFF1-FBE23CF3F9BB}">
   <dimension ref="A3:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K127" sqref="K127"/>
     </sheetView>
   </sheetViews>
@@ -2795,15 +3076,10 @@
       <c r="A5" s="2">
         <v>1103</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
@@ -2811,15 +3087,10 @@
       <c r="A6" s="2">
         <v>1303</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
     </row>
@@ -2827,15 +3098,10 @@
       <c r="A7" s="2">
         <v>1304</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
     </row>
@@ -2843,15 +3109,10 @@
       <c r="A8" s="2">
         <v>1313</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
     </row>
@@ -2859,15 +3120,10 @@
       <c r="A9" s="2">
         <v>1402</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
@@ -2875,15 +3131,10 @@
       <c r="A10" s="2">
         <v>1409</v>
       </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
@@ -2891,15 +3142,10 @@
       <c r="A11" s="2">
         <v>1454</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>
@@ -2907,15 +3153,10 @@
       <c r="A12" s="2">
         <v>1460</v>
       </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
     </row>
@@ -2923,15 +3164,10 @@
       <c r="A13" s="2">
         <v>1466</v>
       </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>1</v>
       </c>
     </row>
@@ -2939,15 +3175,10 @@
       <c r="A14" s="2">
         <v>1473</v>
       </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
     </row>
@@ -2955,15 +3186,10 @@
       <c r="A15" s="2">
         <v>1474</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>1</v>
       </c>
     </row>
@@ -2971,15 +3197,10 @@
       <c r="A16" s="2">
         <v>1477</v>
       </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
@@ -2987,15 +3208,10 @@
       <c r="A17" s="2">
         <v>1504</v>
       </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
     </row>
@@ -3003,15 +3219,10 @@
       <c r="A18" s="2">
         <v>1532</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
     </row>
@@ -3019,15 +3230,10 @@
       <c r="A19" s="2">
         <v>1560</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>1</v>
       </c>
     </row>
@@ -3035,15 +3241,10 @@
       <c r="A20" s="2">
         <v>1718</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="H20">
         <v>1</v>
       </c>
     </row>
@@ -3051,15 +3252,10 @@
       <c r="A21" s="2">
         <v>1734</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
     </row>
@@ -3067,15 +3263,10 @@
       <c r="A22" s="2">
         <v>1784</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>1</v>
       </c>
     </row>
@@ -3083,15 +3274,10 @@
       <c r="A23" s="2">
         <v>1904</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
     </row>
@@ -3099,15 +3285,10 @@
       <c r="A24" s="2">
         <v>2049</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
     </row>
@@ -3115,15 +3296,10 @@
       <c r="A25" s="2">
         <v>2201</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <v>1</v>
       </c>
     </row>
@@ -3131,15 +3307,10 @@
       <c r="A26" s="2">
         <v>2337</v>
       </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>1</v>
       </c>
     </row>
@@ -3147,15 +3318,10 @@
       <c r="A27" s="2">
         <v>2340</v>
       </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="H27">
         <v>1</v>
       </c>
     </row>
@@ -3163,15 +3329,10 @@
       <c r="A28" s="2">
         <v>2345</v>
       </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>1</v>
       </c>
     </row>
@@ -3179,15 +3340,10 @@
       <c r="A29" s="2">
         <v>2414</v>
       </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
     </row>
@@ -3195,15 +3351,10 @@
       <c r="A30" s="2">
         <v>2425</v>
       </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="H30">
         <v>1</v>
       </c>
     </row>
@@ -3211,15 +3362,10 @@
       <c r="A31" s="2">
         <v>2454</v>
       </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="H31">
         <v>1</v>
       </c>
     </row>
@@ -3227,15 +3373,10 @@
       <c r="A32" s="2">
         <v>2464</v>
       </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>1</v>
       </c>
     </row>
@@ -3243,15 +3384,10 @@
       <c r="A33" s="2">
         <v>2468</v>
       </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="H33">
         <v>1</v>
       </c>
     </row>
@@ -3259,15 +3395,10 @@
       <c r="A34" s="2">
         <v>2480</v>
       </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="H34">
         <v>1</v>
       </c>
     </row>
@@ -3275,15 +3406,10 @@
       <c r="A35" s="2">
         <v>2489</v>
       </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="H35">
         <v>1</v>
       </c>
     </row>
@@ -3291,15 +3417,10 @@
       <c r="A36" s="2">
         <v>2515</v>
       </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="H36">
         <v>1</v>
       </c>
     </row>
@@ -3307,15 +3428,10 @@
       <c r="A37" s="2">
         <v>2607</v>
       </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="H37">
         <v>1</v>
       </c>
     </row>
@@ -3323,15 +3439,10 @@
       <c r="A38" s="2">
         <v>2609</v>
       </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="H38">
         <v>1</v>
       </c>
     </row>
@@ -3339,15 +3450,10 @@
       <c r="A39" s="2">
         <v>2618</v>
       </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="H39">
         <v>1</v>
       </c>
     </row>
@@ -3355,15 +3461,10 @@
       <c r="A40" s="2">
         <v>2801</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="H40">
         <v>1</v>
       </c>
     </row>
@@ -3371,15 +3472,10 @@
       <c r="A41" s="2">
         <v>2812</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3">
-        <v>1</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="H41">
         <v>1</v>
       </c>
     </row>
@@ -3387,15 +3483,10 @@
       <c r="A42" s="2">
         <v>2834</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>1</v>
       </c>
     </row>
@@ -3403,15 +3494,10 @@
       <c r="A43" s="2">
         <v>2855</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3">
-        <v>1</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="H43">
         <v>1</v>
       </c>
     </row>
@@ -3419,15 +3505,10 @@
       <c r="A44" s="2">
         <v>2880</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3">
-        <v>1</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="H44">
         <v>1</v>
       </c>
     </row>
@@ -3435,15 +3516,10 @@
       <c r="A45" s="2">
         <v>2881</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3">
-        <v>1</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="H45">
         <v>1</v>
       </c>
     </row>
@@ -3451,15 +3527,10 @@
       <c r="A46" s="2">
         <v>2882</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="H46">
         <v>1</v>
       </c>
     </row>
@@ -3467,15 +3538,10 @@
       <c r="A47" s="2">
         <v>2883</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3">
-        <v>1</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="H47">
         <v>1</v>
       </c>
     </row>
@@ -3483,15 +3549,10 @@
       <c r="A48" s="2">
         <v>2884</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3">
-        <v>1</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="H48">
         <v>1</v>
       </c>
     </row>
@@ -3499,15 +3560,10 @@
       <c r="A49" s="2">
         <v>2885</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3">
-        <v>1</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="H49">
         <v>1</v>
       </c>
     </row>
@@ -3515,15 +3571,10 @@
       <c r="A50" s="2">
         <v>2886</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3">
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="H50">
         <v>1</v>
       </c>
     </row>
@@ -3531,15 +3582,10 @@
       <c r="A51" s="2">
         <v>2887</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3">
-        <v>1</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="H51">
         <v>1</v>
       </c>
     </row>
@@ -3547,15 +3593,10 @@
       <c r="A52" s="2">
         <v>2888</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3">
-        <v>1</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="H52">
         <v>1</v>
       </c>
     </row>
@@ -3563,15 +3604,10 @@
       <c r="A53" s="2">
         <v>2889</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3">
-        <v>1</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="H53">
         <v>1</v>
       </c>
     </row>
@@ -3579,15 +3615,10 @@
       <c r="A54" s="2">
         <v>2890</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3">
-        <v>1</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="H54">
         <v>1</v>
       </c>
     </row>
@@ -3595,15 +3626,10 @@
       <c r="A55" s="2">
         <v>2891</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="H55">
         <v>1</v>
       </c>
     </row>
@@ -3611,15 +3637,10 @@
       <c r="A56" s="2">
         <v>2892</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3">
-        <v>1</v>
-      </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="H56">
         <v>1</v>
       </c>
     </row>
@@ -3627,15 +3648,10 @@
       <c r="A57" s="2">
         <v>2903</v>
       </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="H57">
         <v>1</v>
       </c>
     </row>
@@ -3643,15 +3659,10 @@
       <c r="A58" s="2">
         <v>2936</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="H58">
         <v>1</v>
       </c>
     </row>
@@ -3659,15 +3670,10 @@
       <c r="A59" s="2">
         <v>3005</v>
       </c>
-      <c r="B59" s="3">
-        <v>1</v>
-      </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="H59">
         <v>1</v>
       </c>
     </row>
@@ -3675,15 +3681,10 @@
       <c r="A60" s="2">
         <v>3025</v>
       </c>
-      <c r="B60" s="3">
-        <v>1</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="H60">
         <v>1</v>
       </c>
     </row>
@@ -3691,15 +3692,10 @@
       <c r="A61" s="2">
         <v>3029</v>
       </c>
-      <c r="B61" s="3">
-        <v>1</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="H61">
         <v>1</v>
       </c>
     </row>
@@ -3707,15 +3703,10 @@
       <c r="A62" s="2">
         <v>3044</v>
       </c>
-      <c r="B62" s="3">
-        <v>1</v>
-      </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="H62">
         <v>1</v>
       </c>
     </row>
@@ -3723,15 +3714,10 @@
       <c r="A63" s="2">
         <v>3045</v>
       </c>
-      <c r="B63" s="3">
-        <v>1</v>
-      </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="H63">
         <v>1</v>
       </c>
     </row>
@@ -3739,15 +3725,10 @@
       <c r="A64" s="2">
         <v>3147</v>
       </c>
-      <c r="B64" s="3">
-        <v>1</v>
-      </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="H64">
         <v>1</v>
       </c>
     </row>
@@ -3755,15 +3736,10 @@
       <c r="A65" s="2">
         <v>3163</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3">
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="H65">
         <v>1</v>
       </c>
     </row>
@@ -3771,15 +3747,10 @@
       <c r="A66" s="2">
         <v>3211</v>
       </c>
-      <c r="B66" s="3">
-        <v>1</v>
-      </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="H66">
         <v>1</v>
       </c>
     </row>
@@ -3787,15 +3758,10 @@
       <c r="A67" s="2">
         <v>3297</v>
       </c>
-      <c r="B67" s="3">
-        <v>1</v>
-      </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="H67">
         <v>1</v>
       </c>
     </row>
@@ -3803,15 +3769,10 @@
       <c r="A68" s="2">
         <v>3406</v>
       </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3">
-        <v>1</v>
-      </c>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3">
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="H68">
         <v>1</v>
       </c>
     </row>
@@ -3819,15 +3780,10 @@
       <c r="A69" s="2">
         <v>3434</v>
       </c>
-      <c r="B69" s="3">
-        <v>1</v>
-      </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="H69">
         <v>1</v>
       </c>
     </row>
@@ -3835,15 +3791,10 @@
       <c r="A70" s="2">
         <v>3465</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3">
-        <v>1</v>
-      </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3">
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="H70">
         <v>1</v>
       </c>
     </row>
@@ -3851,15 +3802,10 @@
       <c r="A71" s="2">
         <v>3481</v>
       </c>
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3">
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="H71">
         <v>1</v>
       </c>
     </row>
@@ -3867,15 +3813,10 @@
       <c r="A72" s="2">
         <v>3483</v>
       </c>
-      <c r="B72" s="3">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="H72">
         <v>1</v>
       </c>
     </row>
@@ -3883,15 +3824,10 @@
       <c r="A73" s="2">
         <v>3529</v>
       </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3">
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="H73">
         <v>1</v>
       </c>
     </row>
@@ -3899,15 +3835,10 @@
       <c r="A74" s="2">
         <v>3535</v>
       </c>
-      <c r="B74" s="3">
-        <v>1</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="H74">
         <v>1</v>
       </c>
     </row>
@@ -3915,15 +3846,10 @@
       <c r="A75" s="2">
         <v>3545</v>
       </c>
-      <c r="B75" s="3">
-        <v>1</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="H75">
         <v>1</v>
       </c>
     </row>
@@ -3931,15 +3857,10 @@
       <c r="A76" s="2">
         <v>3552</v>
       </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3">
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="H76">
         <v>1</v>
       </c>
     </row>
@@ -3947,15 +3868,10 @@
       <c r="A77" s="2">
         <v>3563</v>
       </c>
-      <c r="B77" s="3">
-        <v>1</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="H77">
         <v>1</v>
       </c>
     </row>
@@ -3963,15 +3879,10 @@
       <c r="A78" s="2">
         <v>3645</v>
       </c>
-      <c r="B78" s="3">
-        <v>1</v>
-      </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="H78">
         <v>1</v>
       </c>
     </row>
@@ -3979,15 +3890,10 @@
       <c r="A79" s="2">
         <v>3652</v>
       </c>
-      <c r="B79" s="3">
-        <v>1</v>
-      </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="H79">
         <v>1</v>
       </c>
     </row>
@@ -3995,15 +3901,10 @@
       <c r="A80" s="2">
         <v>3687</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3">
-        <v>1</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3">
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="H80">
         <v>1</v>
       </c>
     </row>
@@ -4011,15 +3912,10 @@
       <c r="A81" s="2">
         <v>3702</v>
       </c>
-      <c r="B81" s="3">
-        <v>1</v>
-      </c>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="H81">
         <v>1</v>
       </c>
     </row>
@@ -4027,15 +3923,10 @@
       <c r="A82" s="2">
         <v>3706</v>
       </c>
-      <c r="B82" s="3">
-        <v>1</v>
-      </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="H82">
         <v>1</v>
       </c>
     </row>
@@ -4043,15 +3934,10 @@
       <c r="A83" s="2">
         <v>3708</v>
       </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3">
-        <v>1</v>
-      </c>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3">
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="H83">
         <v>1</v>
       </c>
     </row>
@@ -4059,15 +3945,10 @@
       <c r="A84" s="2">
         <v>4188</v>
       </c>
-      <c r="B84" s="3">
-        <v>1</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3">
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="H84">
         <v>1</v>
       </c>
     </row>
@@ -4075,15 +3956,10 @@
       <c r="A85" s="2">
         <v>4433</v>
       </c>
-      <c r="B85" s="3">
-        <v>1</v>
-      </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="H85">
         <v>1</v>
       </c>
     </row>
@@ -4091,15 +3967,10 @@
       <c r="A86" s="2">
         <v>4534</v>
       </c>
-      <c r="B86" s="3">
-        <v>1</v>
-      </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="H86">
         <v>1</v>
       </c>
     </row>
@@ -4107,15 +3978,10 @@
       <c r="A87" s="2">
         <v>4536</v>
       </c>
-      <c r="B87" s="3">
-        <v>1</v>
-      </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="H87">
         <v>1</v>
       </c>
     </row>
@@ -4123,15 +3989,10 @@
       <c r="A88" s="2">
         <v>4721</v>
       </c>
-      <c r="B88" s="3">
-        <v>1</v>
-      </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="H88">
         <v>1</v>
       </c>
     </row>
@@ -4139,15 +4000,10 @@
       <c r="A89" s="2">
         <v>4971</v>
       </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3">
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="H89">
         <v>1</v>
       </c>
     </row>
@@ -4155,15 +4011,10 @@
       <c r="A90" s="2">
         <v>4979</v>
       </c>
-      <c r="B90" s="3">
-        <v>1</v>
-      </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="H90">
         <v>1</v>
       </c>
     </row>
@@ -4171,15 +4022,10 @@
       <c r="A91" s="2">
         <v>5202</v>
       </c>
-      <c r="B91" s="3">
-        <v>1</v>
-      </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3">
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="H91">
         <v>1</v>
       </c>
     </row>
@@ -4187,15 +4033,10 @@
       <c r="A92" s="2">
         <v>5278</v>
       </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3">
-        <v>1</v>
-      </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3">
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="H92">
         <v>1</v>
       </c>
     </row>
@@ -4203,15 +4044,10 @@
       <c r="A93" s="2">
         <v>5288</v>
       </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3">
-        <v>1</v>
-      </c>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3">
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="H93">
         <v>1</v>
       </c>
     </row>
@@ -4219,15 +4055,10 @@
       <c r="A94" s="2">
         <v>5328</v>
       </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3">
-        <v>1</v>
-      </c>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3">
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="H94">
         <v>1</v>
       </c>
     </row>
@@ -4235,15 +4066,10 @@
       <c r="A95" s="2">
         <v>5347</v>
       </c>
-      <c r="B95" s="3">
-        <v>1</v>
-      </c>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3">
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="H95">
         <v>1</v>
       </c>
     </row>
@@ -4251,15 +4077,10 @@
       <c r="A96" s="2">
         <v>5371</v>
       </c>
-      <c r="B96" s="3">
-        <v>1</v>
-      </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="H96">
         <v>1</v>
       </c>
     </row>
@@ -4267,15 +4088,10 @@
       <c r="A97" s="2">
         <v>5609</v>
       </c>
-      <c r="B97" s="3">
-        <v>1</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3">
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="H97">
         <v>1</v>
       </c>
     </row>
@@ -4283,15 +4099,10 @@
       <c r="A98" s="2">
         <v>5703</v>
       </c>
-      <c r="B98" s="3">
-        <v>1</v>
-      </c>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3">
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="H98">
         <v>1</v>
       </c>
     </row>
@@ -4299,15 +4110,10 @@
       <c r="A99" s="2">
         <v>5876</v>
       </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3">
-        <v>1</v>
-      </c>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
-      <c r="H99" s="3">
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="H99">
         <v>1</v>
       </c>
     </row>
@@ -4315,15 +4121,10 @@
       <c r="A100" s="2">
         <v>5880</v>
       </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3">
-        <v>1</v>
-      </c>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3">
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="H100">
         <v>1</v>
       </c>
     </row>
@@ -4331,15 +4132,10 @@
       <c r="A101" s="2">
         <v>5903</v>
       </c>
-      <c r="B101" s="3">
-        <v>1</v>
-      </c>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3">
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="H101">
         <v>1</v>
       </c>
     </row>
@@ -4347,15 +4143,10 @@
       <c r="A102" s="2">
         <v>6015</v>
       </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3">
-        <v>1</v>
-      </c>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3">
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="H102">
         <v>1</v>
       </c>
     </row>
@@ -4363,15 +4154,10 @@
       <c r="A103" s="2">
         <v>6023</v>
       </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3">
-        <v>1</v>
-      </c>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3">
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="H103">
         <v>1</v>
       </c>
     </row>
@@ -4379,15 +4165,10 @@
       <c r="A104" s="2">
         <v>6112</v>
       </c>
-      <c r="B104" s="3">
-        <v>1</v>
-      </c>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="H104">
         <v>1</v>
       </c>
     </row>
@@ -4395,15 +4176,10 @@
       <c r="A105" s="2">
         <v>6173</v>
       </c>
-      <c r="B105" s="3">
-        <v>1</v>
-      </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="3">
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="H105">
         <v>1</v>
       </c>
     </row>
@@ -4411,15 +4187,10 @@
       <c r="A106" s="2">
         <v>6183</v>
       </c>
-      <c r="B106" s="3">
-        <v>1</v>
-      </c>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3">
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="H106">
         <v>1</v>
       </c>
     </row>
@@ -4427,15 +4198,10 @@
       <c r="A107" s="2">
         <v>6203</v>
       </c>
-      <c r="B107" s="3">
-        <v>1</v>
-      </c>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3">
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="H107">
         <v>1</v>
       </c>
     </row>
@@ -4443,15 +4209,10 @@
       <c r="A108" s="2">
         <v>6204</v>
       </c>
-      <c r="B108" s="3">
-        <v>1</v>
-      </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3">
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="H108">
         <v>1</v>
       </c>
     </row>
@@ -4459,15 +4220,10 @@
       <c r="A109" s="2">
         <v>6214</v>
       </c>
-      <c r="B109" s="3">
-        <v>1</v>
-      </c>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3">
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="H109">
         <v>1</v>
       </c>
     </row>
@@ -4475,15 +4231,10 @@
       <c r="A110" s="2">
         <v>6216</v>
       </c>
-      <c r="B110" s="3">
-        <v>1</v>
-      </c>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3">
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="H110">
         <v>1</v>
       </c>
     </row>
@@ -4491,15 +4242,10 @@
       <c r="A111" s="2">
         <v>6218</v>
       </c>
-      <c r="B111" s="3">
-        <v>1</v>
-      </c>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3">
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="H111">
         <v>1</v>
       </c>
     </row>
@@ -4507,15 +4253,10 @@
       <c r="A112" s="2">
         <v>6220</v>
       </c>
-      <c r="B112" s="3">
-        <v>1</v>
-      </c>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="3"/>
-      <c r="G112" s="3"/>
-      <c r="H112" s="3">
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="H112">
         <v>1</v>
       </c>
     </row>
@@ -4523,15 +4264,10 @@
       <c r="A113" s="2">
         <v>6221</v>
       </c>
-      <c r="B113" s="3">
-        <v>1</v>
-      </c>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3">
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="H113">
         <v>1</v>
       </c>
     </row>
@@ -4539,15 +4275,10 @@
       <c r="A114" s="2">
         <v>6263</v>
       </c>
-      <c r="B114" s="3">
-        <v>1</v>
-      </c>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
-      <c r="H114" s="3">
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="H114">
         <v>1</v>
       </c>
     </row>
@@ -4555,15 +4286,10 @@
       <c r="A115" s="2">
         <v>6277</v>
       </c>
-      <c r="B115" s="3">
-        <v>1</v>
-      </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3">
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="H115">
         <v>1</v>
       </c>
     </row>
@@ -4571,15 +4297,10 @@
       <c r="A116" s="2">
         <v>6446</v>
       </c>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3">
-        <v>1</v>
-      </c>
-      <c r="G116" s="3"/>
-      <c r="H116" s="3">
+      <c r="F116">
+        <v>1</v>
+      </c>
+      <c r="H116">
         <v>1</v>
       </c>
     </row>
@@ -4587,15 +4308,10 @@
       <c r="A117" s="2">
         <v>6613</v>
       </c>
-      <c r="B117" s="3">
-        <v>1</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3">
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="H117">
         <v>1</v>
       </c>
     </row>
@@ -4603,15 +4319,10 @@
       <c r="A118" s="2">
         <v>6669</v>
       </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3">
-        <v>1</v>
-      </c>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3">
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="H118">
         <v>1</v>
       </c>
     </row>
@@ -4619,15 +4330,10 @@
       <c r="A119" s="2">
         <v>6689</v>
       </c>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3">
-        <v>1</v>
-      </c>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3">
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="H119">
         <v>1</v>
       </c>
     </row>
@@ -4635,15 +4341,10 @@
       <c r="A120" s="2">
         <v>6697</v>
       </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3">
-        <v>1</v>
-      </c>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3">
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="H120">
         <v>1</v>
       </c>
     </row>
@@ -4651,15 +4352,10 @@
       <c r="A121" s="2">
         <v>6811</v>
       </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3">
-        <v>1</v>
-      </c>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3">
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="H121">
         <v>1</v>
       </c>
     </row>
@@ -4667,15 +4363,10 @@
       <c r="A122" s="2">
         <v>6874</v>
       </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3">
-        <v>1</v>
-      </c>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3">
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="H122">
         <v>1</v>
       </c>
     </row>
@@ -4683,15 +4374,10 @@
       <c r="A123" s="2">
         <v>6916</v>
       </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3">
-        <v>1</v>
-      </c>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3">
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="H123">
         <v>1</v>
       </c>
     </row>
@@ -4699,15 +4385,10 @@
       <c r="A124" s="2">
         <v>8028</v>
       </c>
-      <c r="B124" s="3">
-        <v>1</v>
-      </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3">
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="H124">
         <v>1</v>
       </c>
     </row>
@@ -4715,15 +4396,10 @@
       <c r="A125" s="2">
         <v>8077</v>
       </c>
-      <c r="B125" s="3">
-        <v>1</v>
-      </c>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
-      <c r="H125" s="3">
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="H125">
         <v>1</v>
       </c>
     </row>
@@ -4731,15 +4407,10 @@
       <c r="A126" s="2">
         <v>8099</v>
       </c>
-      <c r="B126" s="3">
-        <v>1</v>
-      </c>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-      <c r="H126" s="3">
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="H126">
         <v>1</v>
       </c>
     </row>
@@ -4747,15 +4418,10 @@
       <c r="A127" s="2">
         <v>8103</v>
       </c>
-      <c r="B127" s="3">
-        <v>1</v>
-      </c>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
-      <c r="H127" s="3">
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="H127">
         <v>1</v>
       </c>
     </row>
@@ -4763,15 +4429,10 @@
       <c r="A128" s="2">
         <v>8234</v>
       </c>
-      <c r="B128" s="3">
-        <v>1</v>
-      </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3">
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="H128">
         <v>1</v>
       </c>
     </row>
@@ -4779,15 +4440,10 @@
       <c r="A129" s="2">
         <v>8411</v>
       </c>
-      <c r="B129" s="3">
-        <v>1</v>
-      </c>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
-      <c r="H129" s="3">
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="H129">
         <v>1</v>
       </c>
     </row>
@@ -4795,15 +4451,10 @@
       <c r="A130" s="2">
         <v>8916</v>
       </c>
-      <c r="B130" s="3">
-        <v>1</v>
-      </c>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="3"/>
-      <c r="H130" s="3">
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="H130">
         <v>1</v>
       </c>
     </row>
@@ -4811,15 +4462,10 @@
       <c r="A131" s="2">
         <v>9904</v>
       </c>
-      <c r="B131" s="3">
-        <v>1</v>
-      </c>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
-      <c r="G131" s="3"/>
-      <c r="H131" s="3">
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="H131">
         <v>1</v>
       </c>
     </row>
@@ -4827,15 +4473,10 @@
       <c r="A132" s="2">
         <v>9933</v>
       </c>
-      <c r="B132" s="3">
-        <v>1</v>
-      </c>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
-      <c r="G132" s="3"/>
-      <c r="H132" s="3">
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="H132">
         <v>1</v>
       </c>
     </row>
@@ -4843,35 +4484,27 @@
       <c r="A133" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
-      <c r="F133" s="3"/>
-      <c r="G133" s="3"/>
-      <c r="H133" s="3"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B134" s="3">
+      <c r="B134">
         <v>86</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C134">
         <v>21</v>
       </c>
-      <c r="D134" s="3">
+      <c r="D134">
         <v>5</v>
       </c>
-      <c r="E134" s="3">
+      <c r="E134">
         <v>7</v>
       </c>
-      <c r="F134" s="3">
+      <c r="F134">
         <v>9</v>
       </c>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3">
+      <c r="H134">
         <v>128</v>
       </c>
     </row>
@@ -4882,6 +4515,727 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D9FD1E-25F5-4B77-9485-21162AA570DD}">
+  <dimension ref="A1:D87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4966</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5285</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5388</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>8176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4904</v>
+      </c>
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3234</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5353</v>
+      </c>
+      <c r="B9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4908</v>
+      </c>
+      <c r="B10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2444</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3019</v>
+      </c>
+      <c r="B12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2429</v>
+      </c>
+      <c r="B13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6560</v>
+      </c>
+      <c r="B14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2409</v>
+      </c>
+      <c r="B15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8049</v>
+      </c>
+      <c r="B16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3615</v>
+      </c>
+      <c r="B17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6281</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2347</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4994</v>
+      </c>
+      <c r="B21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5203</v>
+      </c>
+      <c r="B22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2427</v>
+      </c>
+      <c r="B23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8416</v>
+      </c>
+      <c r="B24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5210</v>
+      </c>
+      <c r="B25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2453</v>
+      </c>
+      <c r="B26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>4953</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>5403</v>
+      </c>
+      <c r="B28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5410</v>
+      </c>
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>6123</v>
+      </c>
+      <c r="B30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2915</v>
+      </c>
+      <c r="B31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>2207</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2484</v>
+      </c>
+      <c r="B34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>6290</v>
+      </c>
+      <c r="B35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8091</v>
+      </c>
+      <c r="B36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3229</v>
+      </c>
+      <c r="B37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3653</v>
+      </c>
+      <c r="B38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>5301</v>
+      </c>
+      <c r="B39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>8043</v>
+      </c>
+      <c r="B40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2729</v>
+      </c>
+      <c r="B41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1301</v>
+      </c>
+      <c r="B42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1437</v>
+      </c>
+      <c r="B43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1314</v>
+      </c>
+      <c r="B44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2348</v>
+      </c>
+      <c r="B45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>5530</v>
+      </c>
+      <c r="B46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1434</v>
+      </c>
+      <c r="B47" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1440</v>
+      </c>
+      <c r="B48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1445</v>
+      </c>
+      <c r="B49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1419</v>
+      </c>
+      <c r="B50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1417</v>
+      </c>
+      <c r="B51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>4401</v>
+      </c>
+      <c r="B52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1446</v>
+      </c>
+      <c r="B53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1457</v>
+      </c>
+      <c r="B54" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1312</v>
+      </c>
+      <c r="B55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>1463</v>
+      </c>
+      <c r="B56" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>5306</v>
+      </c>
+      <c r="B57" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>9921</v>
+      </c>
+      <c r="B58" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2371</v>
+      </c>
+      <c r="B59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>1503</v>
+      </c>
+      <c r="B60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1558</v>
+      </c>
+      <c r="B61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1590</v>
+      </c>
+      <c r="B62" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2235</v>
+      </c>
+      <c r="B63" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>3176</v>
+      </c>
+      <c r="B64" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>4744</v>
+      </c>
+      <c r="B65" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>6615</v>
+      </c>
+      <c r="B66" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>5438</v>
+      </c>
+      <c r="B67" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3017</v>
+      </c>
+      <c r="B68" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>2387</v>
+      </c>
+      <c r="B69" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>3060</v>
+      </c>
+      <c r="B70" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3002</v>
+      </c>
+      <c r="B71" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>6121</v>
+      </c>
+      <c r="B72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>3611</v>
+      </c>
+      <c r="B73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>1569</v>
+      </c>
+      <c r="B74" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2545</v>
+      </c>
+      <c r="B75" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>1722</v>
+      </c>
+      <c r="B76" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>1776</v>
+      </c>
+      <c r="B77" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>6409</v>
+      </c>
+      <c r="B78" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>5225</v>
+      </c>
+      <c r="B79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>8464</v>
+      </c>
+      <c r="B80" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2208</v>
+      </c>
+      <c r="B81" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2610</v>
+      </c>
+      <c r="B82" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2603</v>
+      </c>
+      <c r="B83" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>8367</v>
+      </c>
+      <c r="B84" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>3034</v>
+      </c>
+      <c r="B85" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>3413</v>
+      </c>
+      <c r="B86" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2330</v>
+      </c>
+      <c r="B87" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D20" r:id="rId1" xr:uid="{3E278227-BC16-4AD6-AC19-736DA49A42CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L129"/>
   <sheetViews>
@@ -7154,7 +7508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77090BAD-0AD2-48E5-92F3-A04FC90F3E57}">
   <dimension ref="A1:B99"/>
   <sheetViews>
@@ -7959,7 +8313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AE9BB1-9308-4B4B-9311-FCBB3D898824}">
   <dimension ref="A1:G158"/>
   <sheetViews>

</xml_diff>